<commit_message>
push functional test for mobile and perf test for mobile using apptim
</commit_message>
<xml_diff>
--- a/LogicalandSecurity/SOAR Software Testing Assessment - Logical and Security.xlsx
+++ b/LogicalandSecurity/SOAR Software Testing Assessment - Logical and Security.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Security Issue ID</t>
   </si>
@@ -50,7 +50,10 @@
 During registration process, no sanitization at all</t>
   </si>
   <si>
-    <t>High</t>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Urgent</t>
   </si>
   <si>
     <t>flask app task.py
@@ -75,6 +78,9 @@
   <si>
     <t>/client_registeration
 Weak password policy</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
   <si>
     <t>password is not validated, hence basic password is able to be submitted</t>
@@ -197,10 +203,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -225,7 +231,7 @@
     <xdr:ext cx="2171700" cy="1533525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image2.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -281,7 +287,7 @@
     <xdr:ext cx="2171700" cy="1533525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -629,26 +635,26 @@
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -672,28 +678,28 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>19</v>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -717,28 +723,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -758,35 +764,35 @@
       <c r="Y4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>4.0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -805,32 +811,32 @@
       <c r="Y5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>5.0</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>12</v>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -851,14 +857,14 @@
     </row>
     <row r="7">
       <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="4"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -878,14 +884,14 @@
     </row>
     <row r="8">
       <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -905,14 +911,14 @@
     </row>
     <row r="9">
       <c r="A9" s="4"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -932,14 +938,14 @@
     </row>
     <row r="10">
       <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -959,14 +965,14 @@
     </row>
     <row r="11">
       <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -986,14 +992,14 @@
     </row>
     <row r="12">
       <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1013,14 +1019,14 @@
     </row>
     <row r="13">
       <c r="A13" s="4"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1040,14 +1046,14 @@
     </row>
     <row r="14">
       <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1067,14 +1073,14 @@
     </row>
     <row r="15">
       <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1094,14 +1100,14 @@
     </row>
     <row r="16">
       <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1121,14 +1127,14 @@
     </row>
     <row r="17">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1148,14 +1154,14 @@
     </row>
     <row r="18">
       <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1175,14 +1181,14 @@
     </row>
     <row r="19">
       <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1202,14 +1208,14 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1229,14 +1235,14 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1256,14 +1262,14 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1283,14 +1289,14 @@
     </row>
     <row r="23">
       <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1310,14 +1316,14 @@
     </row>
     <row r="24">
       <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1337,14 +1343,14 @@
     </row>
     <row r="25">
       <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="4"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1364,14 +1370,14 @@
     </row>
     <row r="26">
       <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="4"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1391,14 +1397,14 @@
     </row>
     <row r="27">
       <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
       <c r="J27" s="4"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>

</xml_diff>